<commit_message>
Clear sample data in benchmark template
</commit_message>
<xml_diff>
--- a/templates/benchmark.xlsx
+++ b/templates/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\tagger-benchmark\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B46BCF2-8D92-4C63-B81C-F52C7E2C9175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD8889A-47E0-48B2-81F2-0067526454A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{51E90C68-60F7-4D68-B794-0E813A261920}"/>
   </bookViews>
@@ -50,53 +50,11 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="7">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
+  <futureMetadata name="XLRICHVALUE" count="1">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="2"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="3"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="4"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="5"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="7"/>
         </ext>
       </extLst>
     </bk>
@@ -106,34 +64,16 @@
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="7">
+  <valueMetadata count="1">
     <bk>
       <rc t="2" v="0"/>
-    </bk>
-    <bk>
-      <rc t="2" v="1"/>
-    </bk>
-    <bk>
-      <rc t="2" v="2"/>
-    </bk>
-    <bk>
-      <rc t="2" v="3"/>
-    </bk>
-    <bk>
-      <rc t="2" v="4"/>
-    </bk>
-    <bk>
-      <rc t="2" v="5"/>
-    </bk>
-    <bk>
-      <rc t="2" v="6"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="22">
   <si>
     <t>Gemini 3 Pro</t>
   </si>
@@ -171,42 +111,6 @@
     <t>Deepseek R1 0528</t>
   </si>
   <si>
-    <t>1girl (0.99), dress (0.97), solo (0.95), black_hair (0.91), head_out_of_frame (0.85), jewelry (0.80), necklace (0.80), long_hair (0.75), bare_shoulders (0.67), outdoors (0.64), see-through (0.62), flower (0.60), plant (0.57), long_sleeves (0.54), standing (0.54), grass (0.50), white_dress (0.47), blue_dress (0.45), off_shoulder (0.42)</t>
-  </si>
-  <si>
-    <t>solo (0.96), phone (0.96), 1girl (0.92), holding_phone (0.92), skirt (0.91), holding (0.89), black_footwear (0.89), cellphone (0.87), plant (0.81), standing (0.79), smartphone (0.78), bag (0.74), black_hair (0.74), full_body (0.70), jewelry (0.69), black_skirt (0.67), potted_plant (0.67), black_bag (0.67), boots (0.66), long_sleeves (0.66), earrings (0.62), black_nails (0.60), short_hair (0.60), outdoors (0.57), pants (0.57), jacket (0.53), asian (0.49), closed_mouth (0.47), long_skirt (0.46), jeans (0.43), shirt (0.42), indoors (0.42), hands_up (0.39), nail_polish (0.38), ring (0.38), shoes (0.36), looking_at_viewer (0.36)</t>
-  </si>
-  <si>
-    <t>head_out_of_frame (0.98), phone (0.96), holding_phone (0.88), solo (0.87), jewelry (0.87), necklace (0.85), cellphone (0.85), holding (0.82), pants (0.71), shirt (0.70), male_focus (0.69), long_sleeves (0.69), 1boy (0.67), smartphone (0.61), indoors (0.57), shirt_tucked_in (0.56), selfie (0.53), belt (0.50), beads (0.44), brown_pants (0.40), puffy_long_sleeves (0.40), see-through (0.38), puffy_sleeves (0.38)</t>
-  </si>
-  <si>
-    <t>1girl (0.96), solo (0.94), phone (0.93), holding (0.87), holding_phone (0.83), cellphone (0.77), selfie (0.75), pants (0.75), short_hair (0.64), white_pants (0.63), long_sleeves (0.62), bag (0.59), black_hair (0.54), indoors (0.51), standing (0.45), smartphone (0.45), sleeves_past_wrists (0.42), pink_sweater (0.42), sweater (0.41), hand_up (0.39), shoulder_bag (0.39), shirt (0.38)</t>
-  </si>
-  <si>
-    <t>1girl (0.97), outdoors (0.87), shirt (0.87), skirt (0.86), solo (0.86), black_footwear (0.80), boots (0.77), sky (0.76), fence (0.74), blonde_hair (0.70), black_shirt (0.66), cloud (0.63), t-shirt (0.62), jewelry (0.56), day (0.55), necklace (0.53), short_sleeves (0.52), blue_sky (0.49), white_skirt (0.46), medium_hair (0.45), from_below (0.45), print_shirt (0.42), see-through (0.41), chain-link_fence (0.35)</t>
-  </si>
-  <si>
-    <t>skirt (0.94), solo (0.93), realistic (0.93), jacket (0.90), photorealistic (0.84), 1girl (0.82), outdoors (0.81), socks (0.79), black_hair (0.76), black_footwear (0.73), asian (0.70), white_socks (0.66), short_hair (0.65), shoes (0.65), pleated_skirt (0.65), shirt (0.63), black_skirt (0.63), blue_sky (0.60), shadow (0.59), full_body (0.59), sky (0.58), standing (0.55), day (0.53), yellow_shirt (0.52), long_sleeves (0.46), sweater (0.46), black_jacket (0.40), yellow_sweater (0.38), open_clothes (0.37), open_jacket (0.35), walking (0.35)</t>
-  </si>
-  <si>
-    <t>"Mui..♡"</t>
-  </si>
-  <si>
-    <t>"🩶⌨️🎧💿"</t>
-  </si>
-  <si>
-    <t>"Alternative elf"</t>
-  </si>
-  <si>
-    <t>"💫"</t>
-  </si>
-  <si>
-    <t>"Fashion inspo - crochet maxi skirt"</t>
-  </si>
-  <si>
-    <t>"death by thrifting"</t>
-  </si>
-  <si>
     <t>LLM</t>
   </si>
   <si>
@@ -228,13 +132,13 @@
     <t>Tag in pool but clearly not relevant</t>
   </si>
   <si>
-    <t>Tag hallucinated</t>
-  </si>
-  <si>
     <t>Tag selected only by 20% and relevant</t>
   </si>
   <si>
     <t>Missing gold status tag</t>
+  </si>
+  <si>
+    <t>Tag not in pool (hallucinated)</t>
   </si>
 </sst>
 </file>
@@ -244,7 +148,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -426,40 +330,39 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -468,7 +371,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="171" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -586,32 +489,8 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="8">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
   <rv s="0">
-    <v>0</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>1</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>2</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>3</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>4</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>5</v>
-    <v>5</v>
-  </rv>
-  <rv s="1">
     <v>en-US</v>
     <v>avysyc</v>
     <v>268435456</v>
@@ -637,18 +516,14 @@
     <v>USDLKR</v>
     <v>USD/LKR</v>
   </rv>
-  <rv s="2">
-    <v>6</v>
+  <rv s="1">
+    <v>0</v>
   </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-  </s>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
   <s t="_linkedentitycore">
     <k n="%EntityCulture" t="s"/>
     <k n="%EntityId" t="s"/>
@@ -809,17 +684,6 @@
     </rSty>
   </richStyles>
 </richStyleSheet>
-</file>
-
-<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
-<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rel r:id="rId1"/>
-  <rel r:id="rId2"/>
-  <rel r:id="rId3"/>
-  <rel r:id="rId4"/>
-  <rel r:id="rId5"/>
-  <rel r:id="rId6"/>
-</richValueRels>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1158,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95508BA-720C-4D63-9631-0B46A1BA1653}">
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="H90" sqref="H90"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1173,690 +1037,636 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="6" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+      <c r="A1" s="4"/>
+      <c r="B1" s="17"/>
       <c r="C1"/>
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="5"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="18"/>
       <c r="C2"/>
       <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="18"/>
       <c r="C3"/>
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="18"/>
       <c r="C4"/>
       <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="18"/>
       <c r="C5"/>
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="18"/>
       <c r="C6"/>
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="18"/>
       <c r="C7"/>
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="18"/>
       <c r="C8"/>
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="18"/>
       <c r="C9"/>
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="18"/>
       <c r="C10"/>
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="18"/>
       <c r="C11"/>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="18"/>
       <c r="C12"/>
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="19"/>
       <c r="C13"/>
       <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="6" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="A15" s="4"/>
+      <c r="B15" s="17"/>
       <c r="C15"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="5"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="18"/>
       <c r="C16"/>
       <c r="D16" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="18"/>
       <c r="C17"/>
       <c r="D17" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="18"/>
       <c r="C18"/>
       <c r="D18" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="18"/>
       <c r="C19"/>
       <c r="D19" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="18"/>
       <c r="C20"/>
       <c r="D20" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="18"/>
       <c r="C21"/>
       <c r="D21" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="18"/>
       <c r="C22"/>
       <c r="D22" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="18"/>
       <c r="C23"/>
       <c r="D23" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="18"/>
       <c r="C24"/>
       <c r="D24" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="18"/>
       <c r="C25"/>
       <c r="D25" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="18"/>
       <c r="C26"/>
       <c r="D26" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="19"/>
       <c r="C27"/>
       <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="6" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
+      <c r="A29" s="4"/>
+      <c r="B29" s="17"/>
       <c r="C29"/>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="5"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="18"/>
       <c r="C30"/>
       <c r="D30" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="18"/>
       <c r="C31"/>
       <c r="D31" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="18"/>
       <c r="C32"/>
       <c r="D32" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="18"/>
       <c r="C33"/>
       <c r="D33" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="8"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="18"/>
       <c r="C34"/>
       <c r="D34" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="18"/>
       <c r="C35"/>
       <c r="D35" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="18"/>
       <c r="C36"/>
       <c r="D36" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="8"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="18"/>
       <c r="C37"/>
       <c r="D37" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="18"/>
       <c r="C38"/>
       <c r="D38" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="8"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="18"/>
       <c r="C39"/>
       <c r="D39" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="8"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="18"/>
       <c r="C40"/>
       <c r="D40" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="9"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="19"/>
       <c r="C41"/>
       <c r="D41" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-    </row>
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B43" s="6" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
+      <c r="A43" s="4"/>
+      <c r="B43" s="17"/>
       <c r="C43"/>
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B44" s="5"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="18"/>
       <c r="C44"/>
       <c r="D44" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="8"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="18"/>
       <c r="C45"/>
       <c r="D45" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="8"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="18"/>
       <c r="C46"/>
       <c r="D46" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="8"/>
-      <c r="B47" s="5"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="18"/>
       <c r="C47"/>
       <c r="D47" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="8"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="18"/>
       <c r="C48"/>
       <c r="D48" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="8"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="18"/>
       <c r="C49"/>
       <c r="D49" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="8"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="18"/>
       <c r="C50"/>
       <c r="D50" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="8"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="18"/>
       <c r="C51"/>
       <c r="D51" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="8"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="18"/>
       <c r="C52"/>
       <c r="D52" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="8"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="15"/>
+      <c r="B53" s="18"/>
       <c r="C53"/>
       <c r="D53" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="8"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="15"/>
+      <c r="B54" s="18"/>
       <c r="C54"/>
       <c r="D54" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="9"/>
-      <c r="B55" s="7"/>
+      <c r="A55" s="16"/>
+      <c r="B55" s="19"/>
       <c r="C55"/>
       <c r="D55" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
-    </row>
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B57" s="6" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="A57" s="4"/>
+      <c r="B57" s="17"/>
       <c r="C57"/>
       <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B58" s="5"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="18"/>
       <c r="C58"/>
       <c r="D58" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="8"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="18"/>
       <c r="C59"/>
       <c r="D59" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="8"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="15"/>
+      <c r="B60" s="18"/>
       <c r="C60"/>
       <c r="D60" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="8"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="15"/>
+      <c r="B61" s="18"/>
       <c r="C61"/>
       <c r="D61" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="8"/>
-      <c r="B62" s="5"/>
+      <c r="A62" s="15"/>
+      <c r="B62" s="18"/>
       <c r="C62"/>
       <c r="D62" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="8"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="18"/>
       <c r="C63"/>
       <c r="D63" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="8"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="15"/>
+      <c r="B64" s="18"/>
       <c r="C64"/>
       <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="8"/>
-      <c r="B65" s="5"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="18"/>
       <c r="C65"/>
       <c r="D65" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="8"/>
-      <c r="B66" s="5"/>
+      <c r="A66" s="15"/>
+      <c r="B66" s="18"/>
       <c r="C66"/>
       <c r="D66" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="8"/>
-      <c r="B67" s="5"/>
+      <c r="A67" s="15"/>
+      <c r="B67" s="18"/>
       <c r="C67"/>
       <c r="D67" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="8"/>
-      <c r="B68" s="5"/>
+      <c r="A68" s="15"/>
+      <c r="B68" s="18"/>
       <c r="C68"/>
       <c r="D68" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="9"/>
-      <c r="B69" s="7"/>
+      <c r="A69" s="16"/>
+      <c r="B69" s="19"/>
       <c r="C69"/>
       <c r="D69" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
-    </row>
+    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="71" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B71" s="6" t="e" vm="6">
-        <v>#VALUE!</v>
-      </c>
+      <c r="A71" s="4"/>
+      <c r="B71" s="17"/>
       <c r="C71"/>
       <c r="D71" s="3"/>
     </row>
     <row r="72" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B72" s="5"/>
+      <c r="A72" s="15"/>
+      <c r="B72" s="18"/>
       <c r="C72"/>
       <c r="D72" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="8"/>
-      <c r="B73" s="5"/>
+      <c r="A73" s="15"/>
+      <c r="B73" s="18"/>
       <c r="C73"/>
       <c r="D73" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="8"/>
-      <c r="B74" s="5"/>
+      <c r="A74" s="15"/>
+      <c r="B74" s="18"/>
       <c r="C74"/>
       <c r="D74" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="8"/>
-      <c r="B75" s="5"/>
+      <c r="A75" s="15"/>
+      <c r="B75" s="18"/>
       <c r="C75"/>
       <c r="D75" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="8"/>
-      <c r="B76" s="5"/>
+      <c r="A76" s="15"/>
+      <c r="B76" s="18"/>
       <c r="C76"/>
       <c r="D76" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="8"/>
-      <c r="B77" s="5"/>
+      <c r="A77" s="15"/>
+      <c r="B77" s="18"/>
       <c r="C77"/>
       <c r="D77" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="8"/>
-      <c r="B78" s="5"/>
+      <c r="A78" s="15"/>
+      <c r="B78" s="18"/>
       <c r="C78"/>
       <c r="D78" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="8"/>
-      <c r="B79" s="5"/>
+      <c r="A79" s="15"/>
+      <c r="B79" s="18"/>
       <c r="C79"/>
       <c r="D79" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="8"/>
-      <c r="B80" s="5"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="18"/>
       <c r="C80"/>
       <c r="D80" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="8"/>
-      <c r="B81" s="5"/>
+      <c r="A81" s="15"/>
+      <c r="B81" s="18"/>
       <c r="C81"/>
       <c r="D81" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="8"/>
-      <c r="B82" s="5"/>
+      <c r="A82" s="15"/>
+      <c r="B82" s="18"/>
       <c r="C82"/>
       <c r="D82" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="9"/>
-      <c r="B83" s="7"/>
+      <c r="A83" s="16"/>
+      <c r="B83" s="19"/>
       <c r="C83"/>
       <c r="D83" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4"/>
-    </row>
+    <row r="84" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D86" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E86" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F86" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G86" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1867,18 +1677,18 @@
         <f>SUM(E2:Z2)+SUM(E16:Z16)+SUM(E30:Z30)+SUM(E44:Z44)+SUM(E58:Z58)+SUM(E72:Z72)</f>
         <v>0</v>
       </c>
-      <c r="F87" s="11">
-        <v>0</v>
-      </c>
-      <c r="G87" s="12" cm="1">
+      <c r="F87" s="5">
+        <v>0</v>
+      </c>
+      <c r="G87" s="6" cm="1">
         <f t="array" aca="1" ref="G87" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
         <v>0</v>
       </c>
-      <c r="I87" s="20">
+      <c r="I87" s="13">
         <v>1</v>
       </c>
       <c r="J87" s="14" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="K87" s="14"/>
       <c r="L87" s="14"/>
@@ -1892,18 +1702,18 @@
         <f t="shared" ref="E88:E98" si="0">SUM(E3:Z3)+SUM(E17:Z17)+SUM(E31:Z31)+SUM(E45:Z45)+SUM(E59:Z59)+SUM(E73:Z73)</f>
         <v>0</v>
       </c>
-      <c r="F88" s="11">
-        <v>0</v>
-      </c>
-      <c r="G88" s="12" cm="1">
+      <c r="F88" s="5">
+        <v>0</v>
+      </c>
+      <c r="G88" s="6" cm="1">
         <f t="array" aca="1" ref="G88" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
         <v>0</v>
       </c>
-      <c r="I88" s="13">
+      <c r="I88" s="7">
         <v>0.5</v>
       </c>
       <c r="J88" s="14" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="K88" s="14"/>
       <c r="L88" s="14"/>
@@ -1917,18 +1727,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F89" s="11">
-        <v>0</v>
-      </c>
-      <c r="G89" s="12" cm="1">
+      <c r="F89" s="5">
+        <v>0</v>
+      </c>
+      <c r="G89" s="6" cm="1">
         <f t="array" aca="1" ref="G89" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
         <v>0</v>
       </c>
-      <c r="I89" s="15">
+      <c r="I89" s="8">
         <v>0.5</v>
       </c>
       <c r="J89" s="14" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="K89" s="14"/>
       <c r="L89" s="14"/>
@@ -1942,18 +1752,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F90" s="11">
-        <v>0</v>
-      </c>
-      <c r="G90" s="12" cm="1">
+      <c r="F90" s="5">
+        <v>0</v>
+      </c>
+      <c r="G90" s="6" cm="1">
         <f t="array" aca="1" ref="G90" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
         <v>0</v>
       </c>
-      <c r="I90" s="16">
+      <c r="I90" s="9">
         <v>-0.5</v>
       </c>
       <c r="J90" s="14" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="K90" s="14"/>
       <c r="L90" s="14"/>
@@ -1967,18 +1777,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F91" s="11">
-        <v>0</v>
-      </c>
-      <c r="G91" s="12" cm="1">
+      <c r="F91" s="5">
+        <v>0</v>
+      </c>
+      <c r="G91" s="6" cm="1">
         <f t="array" aca="1" ref="G91" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
         <v>0</v>
       </c>
-      <c r="I91" s="17">
+      <c r="I91" s="10">
         <v>-0.5</v>
       </c>
       <c r="J91" s="14" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="K91" s="14"/>
       <c r="L91" s="14"/>
@@ -1992,18 +1802,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F92" s="11">
-        <v>0</v>
-      </c>
-      <c r="G92" s="12" cm="1">
+      <c r="F92" s="5">
+        <v>0</v>
+      </c>
+      <c r="G92" s="6" cm="1">
         <f t="array" aca="1" ref="G92" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
         <v>0</v>
       </c>
-      <c r="I92" s="18">
+      <c r="I92" s="11">
         <v>-1</v>
       </c>
       <c r="J92" s="14" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="K92" s="14"/>
       <c r="L92" s="14"/>
@@ -2017,10 +1827,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F93" s="11">
-        <v>0</v>
-      </c>
-      <c r="G93" s="12" cm="1">
+      <c r="F93" s="5">
+        <v>0</v>
+      </c>
+      <c r="G93" s="6" cm="1">
         <f t="array" aca="1" ref="G93" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
         <v>0</v>
       </c>
@@ -2033,14 +1843,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F94" s="11">
-        <v>0</v>
-      </c>
-      <c r="G94" s="12" cm="1">
+      <c r="F94" s="5">
+        <v>0</v>
+      </c>
+      <c r="G94" s="6" cm="1">
         <f t="array" aca="1" ref="G94" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
         <v>0</v>
       </c>
-      <c r="I94" s="19" t="e" vm="7">
+      <c r="I94" s="12" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2052,10 +1862,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F95" s="11">
-        <v>0</v>
-      </c>
-      <c r="G95" s="12" cm="1">
+      <c r="F95" s="5">
+        <v>0</v>
+      </c>
+      <c r="G95" s="6" cm="1">
         <f t="array" aca="1" ref="G95" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
         <v>0</v>
       </c>
@@ -2068,10 +1878,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F96" s="11">
-        <v>0</v>
-      </c>
-      <c r="G96" s="12" cm="1">
+      <c r="F96" s="5">
+        <v>0</v>
+      </c>
+      <c r="G96" s="6" cm="1">
         <f t="array" aca="1" ref="G96" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
         <v>0</v>
       </c>
@@ -2084,10 +1894,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F97" s="11">
-        <v>0</v>
-      </c>
-      <c r="G97" s="12" cm="1">
+      <c r="F97" s="5">
+        <v>0</v>
+      </c>
+      <c r="G97" s="6" cm="1">
         <f t="array" aca="1" ref="G97" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
         <v>0</v>
       </c>
@@ -2100,19 +1910,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F98" s="11">
-        <v>0</v>
-      </c>
-      <c r="G98" s="12" cm="1">
+      <c r="F98" s="5">
+        <v>0</v>
+      </c>
+      <c r="G98" s="6" cm="1">
         <f t="array" aca="1" ref="G98" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="J87:M87"/>
-    <mergeCell ref="J88:M88"/>
-    <mergeCell ref="J89:M89"/>
     <mergeCell ref="J90:M90"/>
     <mergeCell ref="J91:M91"/>
     <mergeCell ref="J92:M92"/>
@@ -2128,6 +1935,9 @@
     <mergeCell ref="B43:B55"/>
     <mergeCell ref="B57:B69"/>
     <mergeCell ref="B71:B83"/>
+    <mergeCell ref="J87:M87"/>
+    <mergeCell ref="J88:M88"/>
+    <mergeCell ref="J89:M89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Update system prompt and benchmark templates
</commit_message>
<xml_diff>
--- a/templates/benchmark.xlsx
+++ b/templates/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\tagger-benchmark\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD8889A-47E0-48B2-81F2-0067526454A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2313676E-5C51-4E0E-B5DB-6613D076EF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{51E90C68-60F7-4D68-B794-0E813A261920}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="21">
   <si>
     <t>Gemini 3 Pro</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Deepseek V3 0324</t>
-  </si>
-  <si>
-    <t>Deepseek R1 0528</t>
   </si>
   <si>
     <t>LLM</t>
@@ -687,16 +684,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D8AF116-8C65-460F-B232-25675ED3CEF2}" name="Table1" displayName="Table1" ref="D86:G98" totalsRowShown="0">
-  <autoFilter ref="D86:G98" xr:uid="{2D8AF116-8C65-460F-B232-25675ED3CEF2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D8AF116-8C65-460F-B232-25675ED3CEF2}" name="Table1" displayName="Table1" ref="D80:G91" totalsRowShown="0">
+  <autoFilter ref="D80:G91" xr:uid="{2D8AF116-8C65-460F-B232-25675ED3CEF2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{61382201-9403-49E8-8122-513CEDEFF875}" name="LLM"/>
     <tableColumn id="2" xr3:uid="{F3365D47-C49F-443D-93E9-07C28E79D2A1}" name="Score">
-      <calculatedColumnFormula>SUM(E2:Z2)+SUM(E16:Z16)+SUM(E30:Z30)+SUM(E44:Z44)+SUM(E58:Z58)+SUM(E72:Z72)</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(E2:Z2)+SUM(E15:Z15)+SUM(E28:Z28)+SUM(E41:Z41)+SUM(E54:Z54)+SUM(E67:Z67)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{09071895-9487-4E75-BEAA-348727B82CA7}" name="Cost (USD)" dataDxfId="0" dataCellStyle="Currency"/>
     <tableColumn id="4" xr3:uid="{406643F3-5471-4257-A413-9AB7F0A2A245}" name="Cost (LKR)" dataCellStyle="Comma">
-      <calculatedColumnFormula array="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</calculatedColumnFormula>
+      <calculatedColumnFormula array="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$88,"Price")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1020,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95508BA-720C-4D63-9631-0B46A1BA1653}">
-  <dimension ref="A1:M98"/>
+  <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1123,34 +1120,34 @@
       </c>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="19"/>
       <c r="C12"/>
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="19"/>
-      <c r="C13"/>
-      <c r="D13" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="17"/>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="17"/>
+      <c r="C14"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="18"/>
       <c r="C15"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="18"/>
       <c r="C16"/>
       <c r="D16" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1158,7 +1155,7 @@
       <c r="B17" s="18"/>
       <c r="C17"/>
       <c r="D17" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1166,7 +1163,7 @@
       <c r="B18" s="18"/>
       <c r="C18"/>
       <c r="D18" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1174,7 +1171,7 @@
       <c r="B19" s="18"/>
       <c r="C19"/>
       <c r="D19" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1182,7 +1179,7 @@
       <c r="B20" s="18"/>
       <c r="C20"/>
       <c r="D20" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1190,7 +1187,7 @@
       <c r="B21" s="18"/>
       <c r="C21"/>
       <c r="D21" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1198,7 +1195,7 @@
       <c r="B22" s="18"/>
       <c r="C22"/>
       <c r="D22" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1206,7 +1203,7 @@
       <c r="B23" s="18"/>
       <c r="C23"/>
       <c r="D23" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1214,46 +1211,46 @@
       <c r="B24" s="18"/>
       <c r="C24"/>
       <c r="D24" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="18"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="19"/>
       <c r="C25"/>
       <c r="D25" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
-      <c r="B26" s="18"/>
-      <c r="C26"/>
-      <c r="D26" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="16"/>
-      <c r="B27" s="19"/>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="17"/>
       <c r="C27"/>
-      <c r="D27" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="17"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
+      <c r="B28" s="18"/>
+      <c r="C28"/>
+      <c r="D28" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15"/>
+      <c r="B29" s="18"/>
       <c r="C29"/>
-      <c r="D29" s="3"/>
+      <c r="D29" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15"/>
       <c r="B30" s="18"/>
       <c r="C30"/>
       <c r="D30" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1261,7 +1258,7 @@
       <c r="B31" s="18"/>
       <c r="C31"/>
       <c r="D31" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1269,7 +1266,7 @@
       <c r="B32" s="18"/>
       <c r="C32"/>
       <c r="D32" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1277,7 +1274,7 @@
       <c r="B33" s="18"/>
       <c r="C33"/>
       <c r="D33" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1285,7 +1282,7 @@
       <c r="B34" s="18"/>
       <c r="C34"/>
       <c r="D34" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1293,7 +1290,7 @@
       <c r="B35" s="18"/>
       <c r="C35"/>
       <c r="D35" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1301,7 +1298,7 @@
       <c r="B36" s="18"/>
       <c r="C36"/>
       <c r="D36" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1309,54 +1306,54 @@
       <c r="B37" s="18"/>
       <c r="C37"/>
       <c r="D37" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
-      <c r="B38" s="18"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="19"/>
       <c r="C38"/>
       <c r="D38" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="18"/>
-      <c r="C39"/>
-      <c r="D39" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="18"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4"/>
+      <c r="B40" s="17"/>
       <c r="C40"/>
-      <c r="D40" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="16"/>
-      <c r="B41" s="19"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="18"/>
       <c r="C41"/>
       <c r="D41" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
-      <c r="B43" s="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="15"/>
+      <c r="B42" s="18"/>
+      <c r="C42"/>
+      <c r="D42" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="15"/>
+      <c r="B43" s="18"/>
       <c r="C43"/>
-      <c r="D43" s="3"/>
+      <c r="D43" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="44" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="15"/>
       <c r="B44" s="18"/>
       <c r="C44"/>
       <c r="D44" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1364,7 +1361,7 @@
       <c r="B45" s="18"/>
       <c r="C45"/>
       <c r="D45" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1372,7 +1369,7 @@
       <c r="B46" s="18"/>
       <c r="C46"/>
       <c r="D46" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1380,7 +1377,7 @@
       <c r="B47" s="18"/>
       <c r="C47"/>
       <c r="D47" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1388,7 +1385,7 @@
       <c r="B48" s="18"/>
       <c r="C48"/>
       <c r="D48" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1396,7 +1393,7 @@
       <c r="B49" s="18"/>
       <c r="C49"/>
       <c r="D49" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1404,62 +1401,62 @@
       <c r="B50" s="18"/>
       <c r="C50"/>
       <c r="D50" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="15"/>
-      <c r="B51" s="18"/>
+      <c r="A51" s="16"/>
+      <c r="B51" s="19"/>
       <c r="C51"/>
       <c r="D51" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="15"/>
-      <c r="B52" s="18"/>
-      <c r="C52"/>
-      <c r="D52" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="15"/>
-      <c r="B53" s="18"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4"/>
+      <c r="B53" s="17"/>
       <c r="C53"/>
-      <c r="D53" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="15"/>
       <c r="B54" s="18"/>
       <c r="C54"/>
       <c r="D54" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="16"/>
-      <c r="B55" s="19"/>
+      <c r="A55" s="15"/>
+      <c r="B55" s="18"/>
       <c r="C55"/>
       <c r="D55" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="4"/>
-      <c r="B57" s="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="15"/>
+      <c r="B56" s="18"/>
+      <c r="C56"/>
+      <c r="D56" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="15"/>
+      <c r="B57" s="18"/>
       <c r="C57"/>
-      <c r="D57" s="3"/>
+      <c r="D57" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="58" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="15"/>
       <c r="B58" s="18"/>
       <c r="C58"/>
       <c r="D58" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1467,7 +1464,7 @@
       <c r="B59" s="18"/>
       <c r="C59"/>
       <c r="D59" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1475,7 +1472,7 @@
       <c r="B60" s="18"/>
       <c r="C60"/>
       <c r="D60" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1483,7 +1480,7 @@
       <c r="B61" s="18"/>
       <c r="C61"/>
       <c r="D61" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1491,7 +1488,7 @@
       <c r="B62" s="18"/>
       <c r="C62"/>
       <c r="D62" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1499,445 +1496,381 @@
       <c r="B63" s="18"/>
       <c r="C63"/>
       <c r="D63" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="15"/>
-      <c r="B64" s="18"/>
+      <c r="A64" s="16"/>
+      <c r="B64" s="19"/>
       <c r="C64"/>
       <c r="D64" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="15"/>
-      <c r="B65" s="18"/>
-      <c r="C65"/>
-      <c r="D65" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="15"/>
-      <c r="B66" s="18"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="4"/>
+      <c r="B66" s="17"/>
       <c r="C66"/>
-      <c r="D66" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="15"/>
       <c r="B67" s="18"/>
       <c r="C67"/>
       <c r="D67" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="15"/>
       <c r="B68" s="18"/>
       <c r="C68"/>
       <c r="D68" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="16"/>
-      <c r="B69" s="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="15"/>
+      <c r="B69" s="18"/>
       <c r="C69"/>
       <c r="D69" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="4"/>
-      <c r="B71" s="17"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="15"/>
+      <c r="B70" s="18"/>
+      <c r="C70"/>
+      <c r="D70" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="15"/>
+      <c r="B71" s="18"/>
       <c r="C71"/>
-      <c r="D71" s="3"/>
-    </row>
-    <row r="72" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D71" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="15"/>
       <c r="B72" s="18"/>
       <c r="C72"/>
       <c r="D72" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="15"/>
       <c r="B73" s="18"/>
       <c r="C73"/>
       <c r="D73" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="15"/>
       <c r="B74" s="18"/>
       <c r="C74"/>
       <c r="D74" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="15"/>
       <c r="B75" s="18"/>
       <c r="C75"/>
       <c r="D75" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="15"/>
       <c r="B76" s="18"/>
       <c r="C76"/>
       <c r="D76" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="15"/>
-      <c r="B77" s="18"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="16"/>
+      <c r="B77" s="19"/>
       <c r="C77"/>
       <c r="D77" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D80" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" t="s">
+        <v>13</v>
+      </c>
+      <c r="G80" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D81" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <f>SUM(E2:Z2)+SUM(E15:Z15)+SUM(E28:Z28)+SUM(E41:Z41)+SUM(E54:Z54)+SUM(E67:Z67)</f>
+        <v>0</v>
+      </c>
+      <c r="F81" s="5">
+        <v>0</v>
+      </c>
+      <c r="G81" s="6" cm="1">
+        <f t="array" aca="1" ref="G81" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$88,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I81" s="13">
+        <v>1</v>
+      </c>
+      <c r="J81" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K81" s="14"/>
+      <c r="L81" s="14"/>
+      <c r="M81" s="14"/>
+    </row>
+    <row r="82" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D82" t="s">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <f>SUM(E3:Z3)+SUM(E16:Z16)+SUM(E29:Z29)+SUM(E42:Z42)+SUM(E55:Z55)+SUM(E68:Z68)</f>
+        <v>0</v>
+      </c>
+      <c r="F82" s="5">
+        <v>0</v>
+      </c>
+      <c r="G82" s="6" cm="1">
+        <f t="array" aca="1" ref="G82" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$88,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I82" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J82" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K82" s="14"/>
+      <c r="L82" s="14"/>
+      <c r="M82" s="14"/>
+    </row>
+    <row r="83" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D83" t="s">
+        <v>2</v>
+      </c>
+      <c r="E83">
+        <f>SUM(E4:Z4)+SUM(E17:Z17)+SUM(E30:Z30)+SUM(E43:Z43)+SUM(E56:Z56)+SUM(E69:Z69)</f>
+        <v>0</v>
+      </c>
+      <c r="F83" s="5">
+        <v>0</v>
+      </c>
+      <c r="G83" s="6" cm="1">
+        <f t="array" aca="1" ref="G83" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$88,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I83" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="J83" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K83" s="14"/>
+      <c r="L83" s="14"/>
+      <c r="M83" s="14"/>
+    </row>
+    <row r="84" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D84" t="s">
+        <v>3</v>
+      </c>
+      <c r="E84">
+        <f>SUM(E5:Z5)+SUM(E18:Z18)+SUM(E31:Z31)+SUM(E44:Z44)+SUM(E57:Z57)+SUM(E70:Z70)</f>
+        <v>0</v>
+      </c>
+      <c r="F84" s="5">
+        <v>0</v>
+      </c>
+      <c r="G84" s="6" cm="1">
+        <f t="array" aca="1" ref="G84" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$88,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I84" s="9">
+        <v>-0.5</v>
+      </c>
+      <c r="J84" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
+      <c r="M84" s="14"/>
+    </row>
+    <row r="85" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D85" t="s">
+        <v>4</v>
+      </c>
+      <c r="E85">
+        <f>SUM(E6:Z6)+SUM(E19:Z19)+SUM(E32:Z32)+SUM(E45:Z45)+SUM(E58:Z58)+SUM(E71:Z71)</f>
+        <v>0</v>
+      </c>
+      <c r="F85" s="5">
+        <v>0</v>
+      </c>
+      <c r="G85" s="6" cm="1">
+        <f t="array" aca="1" ref="G85" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$88,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I85" s="10">
+        <v>-0.5</v>
+      </c>
+      <c r="J85" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K85" s="14"/>
+      <c r="L85" s="14"/>
+      <c r="M85" s="14"/>
+    </row>
+    <row r="86" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D86" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="15"/>
-      <c r="B78" s="18"/>
-      <c r="C78"/>
-      <c r="D78" s="2" t="s">
+      <c r="E86">
+        <f>SUM(E7:Z7)+SUM(E20:Z20)+SUM(E33:Z33)+SUM(E46:Z46)+SUM(E59:Z59)+SUM(E72:Z72)</f>
+        <v>0</v>
+      </c>
+      <c r="F86" s="5">
+        <v>0</v>
+      </c>
+      <c r="G86" s="6" cm="1">
+        <f t="array" aca="1" ref="G86" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$88,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I86" s="11">
+        <v>-1</v>
+      </c>
+      <c r="J86" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K86" s="14"/>
+      <c r="L86" s="14"/>
+      <c r="M86" s="14"/>
+    </row>
+    <row r="87" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D87" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="15"/>
-      <c r="B79" s="18"/>
-      <c r="C79"/>
-      <c r="D79" s="2" t="s">
+      <c r="E87">
+        <f>SUM(E8:Z8)+SUM(E21:Z21)+SUM(E34:Z34)+SUM(E47:Z47)+SUM(E60:Z60)+SUM(E73:Z73)</f>
+        <v>0</v>
+      </c>
+      <c r="F87" s="5">
+        <v>0</v>
+      </c>
+      <c r="G87" s="6" cm="1">
+        <f t="array" aca="1" ref="G87" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$88,"Price")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D88" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="15"/>
-      <c r="B80" s="18"/>
-      <c r="C80"/>
-      <c r="D80" s="2" t="s">
+      <c r="E88">
+        <f>SUM(E9:Z9)+SUM(E22:Z22)+SUM(E35:Z35)+SUM(E48:Z48)+SUM(E61:Z61)+SUM(E74:Z74)</f>
+        <v>0</v>
+      </c>
+      <c r="F88" s="5">
+        <v>0</v>
+      </c>
+      <c r="G88" s="6" cm="1">
+        <f t="array" aca="1" ref="G88" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$88,"Price")</f>
+        <v>0</v>
+      </c>
+      <c r="I88" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="89" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D89" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="15"/>
-      <c r="B81" s="18"/>
-      <c r="C81"/>
-      <c r="D81" s="2" t="s">
+      <c r="E89">
+        <f>SUM(E10:Z10)+SUM(E23:Z23)+SUM(E36:Z36)+SUM(E49:Z49)+SUM(E62:Z62)+SUM(E75:Z75)</f>
+        <v>0</v>
+      </c>
+      <c r="F89" s="5">
+        <v>0</v>
+      </c>
+      <c r="G89" s="6" cm="1">
+        <f t="array" aca="1" ref="G89" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$88,"Price")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D90" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="15"/>
-      <c r="B82" s="18"/>
-      <c r="C82"/>
-      <c r="D82" s="2" t="s">
+      <c r="E90">
+        <f>SUM(E11:Z11)+SUM(E24:Z24)+SUM(E37:Z37)+SUM(E50:Z50)+SUM(E63:Z63)+SUM(E76:Z76)</f>
+        <v>0</v>
+      </c>
+      <c r="F90" s="5">
+        <v>0</v>
+      </c>
+      <c r="G90" s="6" cm="1">
+        <f t="array" aca="1" ref="G90" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$88,"Price")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D91" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="16"/>
-      <c r="B83" s="19"/>
-      <c r="C83"/>
-      <c r="D83" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D86" t="s">
-        <v>12</v>
-      </c>
-      <c r="E86" t="s">
-        <v>13</v>
-      </c>
-      <c r="F86" t="s">
-        <v>14</v>
-      </c>
-      <c r="G86" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D87" t="s">
-        <v>0</v>
-      </c>
-      <c r="E87">
-        <f>SUM(E2:Z2)+SUM(E16:Z16)+SUM(E30:Z30)+SUM(E44:Z44)+SUM(E58:Z58)+SUM(E72:Z72)</f>
-        <v>0</v>
-      </c>
-      <c r="F87" s="5">
-        <v>0</v>
-      </c>
-      <c r="G87" s="6" cm="1">
-        <f t="array" aca="1" ref="G87" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
-        <v>0</v>
-      </c>
-      <c r="I87" s="13">
-        <v>1</v>
-      </c>
-      <c r="J87" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="K87" s="14"/>
-      <c r="L87" s="14"/>
-      <c r="M87" s="14"/>
-    </row>
-    <row r="88" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D88" t="s">
-        <v>1</v>
-      </c>
-      <c r="E88">
-        <f t="shared" ref="E88:E98" si="0">SUM(E3:Z3)+SUM(E17:Z17)+SUM(E31:Z31)+SUM(E45:Z45)+SUM(E59:Z59)+SUM(E73:Z73)</f>
-        <v>0</v>
-      </c>
-      <c r="F88" s="5">
-        <v>0</v>
-      </c>
-      <c r="G88" s="6" cm="1">
-        <f t="array" aca="1" ref="G88" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
-        <v>0</v>
-      </c>
-      <c r="I88" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="J88" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="K88" s="14"/>
-      <c r="L88" s="14"/>
-      <c r="M88" s="14"/>
-    </row>
-    <row r="89" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D89" t="s">
-        <v>2</v>
-      </c>
-      <c r="E89">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F89" s="5">
-        <v>0</v>
-      </c>
-      <c r="G89" s="6" cm="1">
-        <f t="array" aca="1" ref="G89" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
-        <v>0</v>
-      </c>
-      <c r="I89" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="J89" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K89" s="14"/>
-      <c r="L89" s="14"/>
-      <c r="M89" s="14"/>
-    </row>
-    <row r="90" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D90" t="s">
-        <v>3</v>
-      </c>
-      <c r="E90">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F90" s="5">
-        <v>0</v>
-      </c>
-      <c r="G90" s="6" cm="1">
-        <f t="array" aca="1" ref="G90" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
-        <v>0</v>
-      </c>
-      <c r="I90" s="9">
-        <v>-0.5</v>
-      </c>
-      <c r="J90" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="K90" s="14"/>
-      <c r="L90" s="14"/>
-      <c r="M90" s="14"/>
-    </row>
-    <row r="91" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D91" t="s">
-        <v>4</v>
-      </c>
       <c r="E91">
-        <f t="shared" si="0"/>
+        <f>SUM(E12:Z12)+SUM(E25:Z25)+SUM(E38:Z38)+SUM(E51:Z51)+SUM(E64:Z64)+SUM(E77:Z77)</f>
         <v>0</v>
       </c>
       <c r="F91" s="5">
         <v>0</v>
       </c>
       <c r="G91" s="6" cm="1">
-        <f t="array" aca="1" ref="G91" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
-        <v>0</v>
-      </c>
-      <c r="I91" s="10">
-        <v>-0.5</v>
-      </c>
-      <c r="J91" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K91" s="14"/>
-      <c r="L91" s="14"/>
-      <c r="M91" s="14"/>
-    </row>
-    <row r="92" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D92" t="s">
-        <v>5</v>
-      </c>
-      <c r="E92">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F92" s="5">
-        <v>0</v>
-      </c>
-      <c r="G92" s="6" cm="1">
-        <f t="array" aca="1" ref="G92" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
-        <v>0</v>
-      </c>
-      <c r="I92" s="11">
-        <v>-1</v>
-      </c>
-      <c r="J92" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="K92" s="14"/>
-      <c r="L92" s="14"/>
-      <c r="M92" s="14"/>
-    </row>
-    <row r="93" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D93" t="s">
-        <v>6</v>
-      </c>
-      <c r="E93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F93" s="5">
-        <v>0</v>
-      </c>
-      <c r="G93" s="6" cm="1">
-        <f t="array" aca="1" ref="G93" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D94" t="s">
-        <v>7</v>
-      </c>
-      <c r="E94">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F94" s="5">
-        <v>0</v>
-      </c>
-      <c r="G94" s="6" cm="1">
-        <f t="array" aca="1" ref="G94" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
-        <v>0</v>
-      </c>
-      <c r="I94" s="12" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D95" t="s">
-        <v>8</v>
-      </c>
-      <c r="E95">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F95" s="5">
-        <v>0</v>
-      </c>
-      <c r="G95" s="6" cm="1">
-        <f t="array" aca="1" ref="G95" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D96" t="s">
-        <v>9</v>
-      </c>
-      <c r="E96">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F96" s="5">
-        <v>0</v>
-      </c>
-      <c r="G96" s="6" cm="1">
-        <f t="array" aca="1" ref="G96" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="4:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D97" t="s">
-        <v>10</v>
-      </c>
-      <c r="E97">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F97" s="5">
-        <v>0</v>
-      </c>
-      <c r="G97" s="6" cm="1">
-        <f t="array" aca="1" ref="G97" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="4:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D98" t="s">
-        <v>11</v>
-      </c>
-      <c r="E98">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F98" s="5">
-        <v>0</v>
-      </c>
-      <c r="G98" s="6" cm="1">
-        <f t="array" aca="1" ref="G98" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$94,"Price")</f>
+        <f t="array" aca="1" ref="G91" ca="1">Table1[[#This Row],[Cost (USD)]]*_FV($I$88,"Price")</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="J90:M90"/>
-    <mergeCell ref="J91:M91"/>
-    <mergeCell ref="J92:M92"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A30:A41"/>
-    <mergeCell ref="A44:A55"/>
-    <mergeCell ref="A58:A69"/>
-    <mergeCell ref="A72:A83"/>
-    <mergeCell ref="B1:B13"/>
-    <mergeCell ref="B15:B27"/>
-    <mergeCell ref="B29:B41"/>
-    <mergeCell ref="B43:B55"/>
-    <mergeCell ref="B57:B69"/>
-    <mergeCell ref="B71:B83"/>
-    <mergeCell ref="J87:M87"/>
-    <mergeCell ref="J88:M88"/>
-    <mergeCell ref="J89:M89"/>
+    <mergeCell ref="J82:M82"/>
+    <mergeCell ref="J83:M83"/>
+    <mergeCell ref="J84:M84"/>
+    <mergeCell ref="J85:M85"/>
+    <mergeCell ref="J86:M86"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="A15:A25"/>
+    <mergeCell ref="A28:A38"/>
+    <mergeCell ref="A41:A51"/>
+    <mergeCell ref="A54:A64"/>
+    <mergeCell ref="A67:A77"/>
+    <mergeCell ref="B1:B12"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="B27:B38"/>
+    <mergeCell ref="B40:B51"/>
+    <mergeCell ref="B53:B64"/>
+    <mergeCell ref="B66:B77"/>
+    <mergeCell ref="J81:M81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>